<commit_message>
Implement parallel processing for CAO analysis with robust duplicate control and Excel merging
- Add parallel processing using multiple Google API keys for 3_llmExtraction.py and 4_analysis.py
- Implement file-level locking to prevent race conditions between parallel processes
- Add process-specific Excel output files with intelligent merging to preserve existing data
- Replace marker-based duplicate detection with Excel-based checking for better data integrity
- Clean up merge logic and remove verbose debug output for cleaner terminal experience
- Fix deprecated boolean inversion operator and CAO ID duplicate checking issues
</commit_message>
<xml_diff>
--- a/inputExcel/250702 AI information matrix.xlsx
+++ b/inputExcel/250702 AI information matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzpiazolo/Documents/Python/CAOsDataExtraction/inputExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D96ACEB-1523-BF41-B1A0-4B277DED6AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922849DA-5F6E-4B42-A5AE-D5D31B2E79BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16020" activeTab="2" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="153">
   <si>
     <t>CAO</t>
   </si>
@@ -485,6 +485,18 @@
   </si>
   <si>
     <t>all information about third jobgroup. Often mentioned in wage table as column titles (number or text). Ex: I=Statutory minimum wage (WML); F-21-5; 65-12-57</t>
+  </si>
+  <si>
+    <t>Homeoffice</t>
+  </si>
+  <si>
+    <t>start date of contract usually on front page (date in dd/mm/yyyy format). Ex: 01/04/2019; 01/01/2017; 01/07/2019</t>
+  </si>
+  <si>
+    <t>end date of contract usually on front page (date in dd/mm/yyyy format). Ex: 31/01/2023; 31/03/2019; 28/02/2015</t>
+  </si>
+  <si>
+    <t>All information related to home office, remote work, or telecommuting (text). Include rules, eligibility, allowance, equipment, and any limitations. Ex: Employees may work from home up to 2 days per week; Home office allowance of €3 per day; Maximum 8 days per month remote work permitted.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +546,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,6 +580,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFBD4B4"/>
+        <bgColor rgb="FFFBD4B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor rgb="FFFBD4B4"/>
       </patternFill>
     </fill>
@@ -619,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -645,6 +663,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,15 +1000,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BF5F48-E2E4-AB45-AC3D-2386CAD72E8A}">
-  <dimension ref="A1:BN10"/>
+  <dimension ref="A1:BO11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" activeCellId="1" sqref="A1:XFD1 A6:XFD10"/>
+    <sheetView topLeftCell="BI1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BP11" sqref="BP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:66" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:67" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1186,8 +1207,11 @@
       <c r="BN1" s="9" t="s">
         <v>56</v>
       </c>
+      <c r="BO1" s="11" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1301,7 +1325,7 @@
       </c>
       <c r="AU2" s="1"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1414,7 +1438,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1527,7 +1551,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1640,7 +1664,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:66" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1672,7 +1696,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1707,7 +1731,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1742,7 +1766,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1777,7 +1801,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1795,6 +1819,26 @@
       </c>
       <c r="BN10" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO11" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2326,15 +2370,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA65DA5-B948-1C47-BC06-E1245285351C}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -2422,8 +2466,11 @@
       <c r="AC1" s="9" t="s">
         <v>56</v>
       </c>
+      <c r="AD1" s="11" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2507,6 +2554,9 @@
       </c>
       <c r="AC2" t="s">
         <v>145</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance LLM extraction and analysis scripts with improved configuration and error handling
- Increased MAX_JSON_FILES limit in both 3_llmExtraction.py and 4_analysis.py to allow processing of more files.
- Introduced MAX_PROCESSING_TIME_HOURS to set a maximum time for processing each file.
- Added SORTED_FILES option to control file order during processing.
- Implemented consistent error logging for failed file extractions and analyses.
- Updated prompts in fields_prompt.md and related files for clarity and consistency.
- Enhanced README.md to reflect changes in workflow and script execution order.
</commit_message>
<xml_diff>
--- a/inputExcel/250702 AI information matrix.xlsx
+++ b/inputExcel/250702 AI information matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzpiazolo/Documents/Python/CAOsDataExtraction/inputExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922849DA-5F6E-4B42-A5AE-D5D31B2E79BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD9D9A-CD43-A249-9E29-AEDF71E9F039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16020" activeTab="2" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="15880" activeTab="2" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="154">
   <si>
     <t>CAO</t>
   </si>
@@ -235,9 +235,6 @@
     <t>File_name</t>
   </si>
   <si>
-    <t>pdf file name (text).</t>
-  </si>
-  <si>
     <t>In pdf file name. (boolean: Yes/No). Ex: Yes; No</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>start date of seventh wage table (date in dd/mm/yyyy format). Ex: 01/01/2018; 01/01/2017; 01/07/2010</t>
   </si>
   <si>
-    <t>Does the CAO file contain additional basic/normal wage tables beyond the 7 already extracted? (Boolean: Yes/No). Ex: Yes; No</t>
-  </si>
-  <si>
     <t>All additional context related to salary interpretation not covered in other fields (text). Ex: Youth salary scales phased out from 2014; Hourly wage = monthly salary / 156; Classification via FWG® system; Introductory salary scales abolished as of 2013</t>
   </si>
   <si>
@@ -497,6 +491,15 @@
   </si>
   <si>
     <t>All information related to home office, remote work, or telecommuting (text). Include rules, eligibility, allowance, equipment, and any limitations. Ex: Employees may work from home up to 2 days per week; Home office allowance of €3 per day; Maximum 8 days per month remote work permitted.</t>
+  </si>
+  <si>
+    <t>Does the CAO file contain additional basic/normal wage tables beyond the 7 already extracted in the precious columns? (Boolean: Yes/No). Ex: Yes; No</t>
+  </si>
+  <si>
+    <t>start date of contract usually under general information (date in dd/mm/yyyy format). Ex: 01/04/2019; 01/01/2017; 01/07/2018</t>
+  </si>
+  <si>
+    <t>end date of contract usually under general information (date in dd/mm/yyyy format). Ex: 31/01/2023; 31/03/2019; 28/02/2014</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BF5F48-E2E4-AB45-AC3D-2386CAD72E8A}">
   <dimension ref="A1:BO11"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BP11" sqref="BP11"/>
+    <sheetView topLeftCell="AH1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL29" sqref="AL29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,10 +1151,10 @@
         <v>42</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AV1" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AW1" s="7" t="s">
         <v>43</v>
@@ -1208,364 +1211,352 @@
         <v>56</v>
       </c>
       <c r="BO1" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" t="s">
-        <v>146</v>
-      </c>
-      <c r="L2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>79</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>80</v>
       </c>
-      <c r="P2" t="s">
-        <v>81</v>
-      </c>
       <c r="Q2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" t="s">
         <v>84</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>85</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>86</v>
       </c>
-      <c r="T2" t="s">
-        <v>87</v>
-      </c>
       <c r="U2" t="s">
+        <v>89</v>
+      </c>
+      <c r="V2" t="s">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>91</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>92</v>
       </c>
-      <c r="X2" t="s">
-        <v>93</v>
-      </c>
       <c r="Y2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" t="s">
         <v>96</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" t="s">
-        <v>99</v>
-      </c>
       <c r="AC2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD2" t="s">
         <v>102</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>103</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>104</v>
       </c>
-      <c r="AF2" t="s">
-        <v>105</v>
-      </c>
       <c r="AG2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH2" t="s">
         <v>108</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>109</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>110</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>111</v>
-      </c>
       <c r="AK2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL2" t="s">
         <v>114</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO2" t="s">
         <v>115</v>
       </c>
-      <c r="AM2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>116</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>118</v>
       </c>
       <c r="AU2" s="1"/>
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" t="s">
         <v>78</v>
       </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" t="s">
-        <v>147</v>
-      </c>
-      <c r="L3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>79</v>
       </c>
-      <c r="O3" t="s">
-        <v>80</v>
-      </c>
       <c r="P3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q3" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" t="s">
         <v>84</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>85</v>
       </c>
-      <c r="S3" t="s">
-        <v>86</v>
-      </c>
       <c r="T3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U3" t="s">
+        <v>89</v>
+      </c>
+      <c r="V3" t="s">
         <v>90</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>91</v>
       </c>
-      <c r="W3" t="s">
-        <v>92</v>
-      </c>
       <c r="X3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z3" t="s">
         <v>96</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>97</v>
       </c>
-      <c r="AA3" t="s">
-        <v>98</v>
-      </c>
       <c r="AB3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD3" t="s">
         <v>102</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>103</v>
       </c>
-      <c r="AE3" t="s">
-        <v>104</v>
-      </c>
       <c r="AF3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH3" t="s">
         <v>108</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>109</v>
       </c>
-      <c r="AI3" t="s">
-        <v>110</v>
-      </c>
       <c r="AJ3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AK3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL3" t="s">
         <v>114</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO3" t="s">
         <v>115</v>
       </c>
-      <c r="AM3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AN3" t="s">
+      <c r="AP3" t="s">
         <v>116</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" t="s">
         <v>78</v>
       </c>
-      <c r="J4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>79</v>
       </c>
-      <c r="O4" t="s">
-        <v>80</v>
-      </c>
       <c r="P4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q4" t="s">
         <v>83</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>84</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>85</v>
       </c>
-      <c r="S4" t="s">
-        <v>86</v>
-      </c>
       <c r="T4" t="s">
+        <v>88</v>
+      </c>
+      <c r="U4" t="s">
         <v>89</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>90</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>91</v>
       </c>
-      <c r="W4" t="s">
-        <v>92</v>
-      </c>
       <c r="X4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" t="s">
         <v>95</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>96</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>97</v>
       </c>
-      <c r="AA4" t="s">
-        <v>98</v>
-      </c>
       <c r="AB4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC4" t="s">
         <v>101</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>102</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>103</v>
       </c>
-      <c r="AE4" t="s">
-        <v>104</v>
-      </c>
       <c r="AF4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG4" t="s">
         <v>107</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>108</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>109</v>
       </c>
-      <c r="AI4" t="s">
-        <v>110</v>
-      </c>
       <c r="AJ4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK4" t="s">
         <v>113</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>114</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO4" t="s">
         <v>115</v>
       </c>
-      <c r="AM4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AN4" t="s">
+      <c r="AP4" t="s">
         <v>116</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" t="s">
         <v>65</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
       </c>
       <c r="K5" t="s">
         <v>61</v>
@@ -1665,180 +1656,162 @@
       </c>
     </row>
     <row r="6" spans="1:67" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" t="s">
-        <v>66</v>
-      </c>
       <c r="AQ6" t="s">
+        <v>118</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT6" t="s">
         <v>120</v>
       </c>
-      <c r="AR6" t="s">
-        <v>125</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>122</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" t="s">
-        <v>66</v>
-      </c>
       <c r="AV7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AW7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>132</v>
+      </c>
+      <c r="BA7" t="s">
         <v>129</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>134</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" t="s">
-        <v>66</v>
-      </c>
       <c r="BB8" t="s">
+        <v>131</v>
+      </c>
+      <c r="BC8" t="s">
         <v>133</v>
       </c>
-      <c r="BC8" t="s">
+      <c r="BD8" t="s">
+        <v>130</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>134</v>
+      </c>
+      <c r="BF8" t="s">
         <v>135</v>
       </c>
-      <c r="BD8" t="s">
-        <v>132</v>
-      </c>
-      <c r="BE8" t="s">
+      <c r="BG8" t="s">
         <v>136</v>
-      </c>
-      <c r="BF8" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" t="s">
-        <v>66</v>
-      </c>
       <c r="BH9" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>138</v>
+      </c>
+      <c r="BJ9" t="s">
         <v>139</v>
       </c>
-      <c r="BI9" t="s">
+      <c r="BK9" t="s">
         <v>140</v>
       </c>
-      <c r="BJ9" t="s">
+      <c r="BL9" t="s">
         <v>141</v>
       </c>
-      <c r="BK9" t="s">
+      <c r="BM9" t="s">
         <v>142</v>
-      </c>
-      <c r="BL9" t="s">
-        <v>143</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" t="s">
-        <v>66</v>
-      </c>
       <c r="BN10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="BO11" t="s">
         <v>150</v>
-      </c>
-      <c r="H11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J11" t="s">
-        <v>66</v>
-      </c>
-      <c r="BO11" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1850,127 +1823,124 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CD2C15-18CD-B441-BAB5-E2EE8A3E9E99}">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>64</v>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG1" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
         <v>79</v>
@@ -1979,7 +1949,7 @@
         <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
         <v>84</v>
@@ -1991,7 +1961,7 @@
         <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L2" t="s">
         <v>90</v>
@@ -2003,7 +1973,7 @@
         <v>92</v>
       </c>
       <c r="O2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P2" t="s">
         <v>96</v>
@@ -2015,7 +1985,7 @@
         <v>98</v>
       </c>
       <c r="S2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="T2" t="s">
         <v>102</v>
@@ -2027,7 +1997,7 @@
         <v>104</v>
       </c>
       <c r="W2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="X2" t="s">
         <v>108</v>
@@ -2039,48 +2009,45 @@
         <v>110</v>
       </c>
       <c r="AA2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AB2" t="s">
         <v>114</v>
       </c>
       <c r="AC2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE2" t="s">
         <v>115</v>
       </c>
-      <c r="AD2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>116</v>
       </c>
-      <c r="AF2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>118</v>
-      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
         <v>84</v>
@@ -2089,10 +2056,10 @@
         <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L3" t="s">
         <v>90</v>
@@ -2101,10 +2068,10 @@
         <v>91</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P3" t="s">
         <v>96</v>
@@ -2113,10 +2080,10 @@
         <v>97</v>
       </c>
       <c r="R3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="T3" t="s">
         <v>102</v>
@@ -2125,10 +2092,10 @@
         <v>103</v>
       </c>
       <c r="V3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="W3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="X3" t="s">
         <v>108</v>
@@ -2137,48 +2104,45 @@
         <v>109</v>
       </c>
       <c r="Z3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AA3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AB3" t="s">
         <v>114</v>
       </c>
       <c r="AC3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE3" t="s">
         <v>115</v>
       </c>
-      <c r="AD3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>116</v>
       </c>
-      <c r="AF3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>118</v>
-      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
         <v>83</v>
@@ -2190,7 +2154,7 @@
         <v>85</v>
       </c>
       <c r="J4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K4" t="s">
         <v>89</v>
@@ -2202,7 +2166,7 @@
         <v>91</v>
       </c>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O4" t="s">
         <v>95</v>
@@ -2214,7 +2178,7 @@
         <v>97</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S4" t="s">
         <v>101</v>
@@ -2226,7 +2190,7 @@
         <v>103</v>
       </c>
       <c r="V4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="W4" t="s">
         <v>107</v>
@@ -2238,7 +2202,7 @@
         <v>109</v>
       </c>
       <c r="Z4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AA4" t="s">
         <v>113</v>
@@ -2247,24 +2211,21 @@
         <v>114</v>
       </c>
       <c r="AC4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE4" t="s">
         <v>115</v>
       </c>
-      <c r="AD4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>116</v>
       </c>
-      <c r="AF4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>118</v>
-      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -2357,9 +2318,6 @@
         <v>61</v>
       </c>
       <c r="AF5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2370,193 +2328,178 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA65DA5-B948-1C47-BC06-E1245285351C}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP5" sqref="AP5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>64</v>
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD1" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
         <v>120</v>
       </c>
       <c r="G2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" t="s">
         <v>125</v>
       </c>
-      <c r="H2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" t="s">
-        <v>126</v>
-      </c>
       <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
         <v>129</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>131</v>
+      </c>
+      <c r="O2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P2" t="s">
         <v>130</v>
       </c>
-      <c r="N2" t="s">
-        <v>127</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>134</v>
-      </c>
-      <c r="P2" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>133</v>
       </c>
       <c r="R2" t="s">
         <v>135</v>
       </c>
       <c r="S2" t="s">
-        <v>132</v>
-      </c>
-      <c r="T2" t="s">
         <v>136</v>
       </c>
+      <c r="T2" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="U2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="V2" t="s">
-        <v>138</v>
-      </c>
-      <c r="W2" s="10" t="s">
         <v>139</v>
       </c>
+      <c r="W2" t="s">
+        <v>140</v>
+      </c>
       <c r="X2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="Y2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Z2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AA2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>